<commit_message>
Consolidating intervention names and adding definitions
</commit_message>
<xml_diff>
--- a/data/dpo_app_data.xlsx
+++ b/data/dpo_app_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="795">
   <si>
     <t xml:space="preserve">study_author_year</t>
   </si>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">15.05 (1.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">UP-A</t>
+    <t xml:space="preserve">Unified Protocol for Transdiagnostic Treatment of Emotional Disorders in Adolescents (UP-A)</t>
   </si>
   <si>
     <t xml:space="preserve">Waitlist</t>
@@ -275,7 +275,7 @@
     <t xml:space="preserve">14.56 (0.97)</t>
   </si>
   <si>
-    <t xml:space="preserve">Experimental Intervention</t>
+    <t xml:space="preserve">"Implicit theory of personality" intervention</t>
   </si>
   <si>
     <t xml:space="preserve">Active: Control intervention</t>
@@ -482,7 +482,7 @@
     <t xml:space="preserve">11.8 (0.7)</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP-A-ASD</t>
+    <t xml:space="preserve">Resourceful Adolescent Program-Autism Spectrum Disorder (RAP-A-ASD)</t>
   </si>
   <si>
     <t xml:space="preserve">6, 7</t>
@@ -723,7 +723,7 @@
     <t xml:space="preserve">13.35 (0.71)</t>
   </si>
   <si>
-    <t xml:space="preserve">OVK; SPARX; OVK &amp; SPARX</t>
+    <t xml:space="preserve">Op Volle Kracht (OVK); SPARX; OVK &amp; SPARX</t>
   </si>
   <si>
     <t xml:space="preserve">100%</t>
@@ -864,9 +864,6 @@
     <t xml:space="preserve">599 students, 3 schools</t>
   </si>
   <si>
-    <t xml:space="preserve">intervention</t>
-  </si>
-  <si>
     <t xml:space="preserve">Active: Control</t>
   </si>
   <si>
@@ -936,7 +933,7 @@
     <t xml:space="preserve">13.42 (0.77)</t>
   </si>
   <si>
-    <t xml:space="preserve">OVK</t>
+    <t xml:space="preserve">Op Volle Kracht (OVK)</t>
   </si>
   <si>
     <t xml:space="preserve">https://pubmed.ncbi.nlm.nih.gov/24837666/</t>
@@ -960,7 +957,7 @@
     <t xml:space="preserve">15.4 (1.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mindfulness condition</t>
+    <t xml:space="preserve">Mindfulness group training</t>
   </si>
   <si>
     <t xml:space="preserve">9, 10, 11, 12</t>
@@ -994,7 +991,7 @@
     <t xml:space="preserve">12.22 (0.77)</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP-PIR</t>
+    <t xml:space="preserve">Resourceful Adolescent Program - Peer Interpersonal Relatedness (RAP-PIR)</t>
   </si>
   <si>
     <t xml:space="preserve">Active: RAP-Placebo program; Waitlist</t>
@@ -1066,7 +1063,7 @@
     <t xml:space="preserve">11.51 (10.91)</t>
   </si>
   <si>
-    <t xml:space="preserve">UKPR</t>
+    <t xml:space="preserve">UK Resilience Programme (UKRP)</t>
   </si>
   <si>
     <t xml:space="preserve">Quasi-experimental design</t>
@@ -1180,7 +1177,7 @@
     <t xml:space="preserve">19 students, 1 schools</t>
   </si>
   <si>
-    <t xml:space="preserve">CWD-A</t>
+    <t xml:space="preserve">Adolescent Coping with Depression (CWD-A)</t>
   </si>
   <si>
     <t xml:space="preserve">5, 6, 7, 8</t>
@@ -1276,7 +1273,7 @@
     <t xml:space="preserve">711 students, 1 schools</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP-UK</t>
+    <t xml:space="preserve">Resourceful Adolescent Program adapted for the UK (RAP-UK)</t>
   </si>
   <si>
     <t xml:space="preserve">Attention Control; TAU</t>
@@ -1438,7 +1435,7 @@
     <t xml:space="preserve">14</t>
   </si>
   <si>
-    <t xml:space="preserve">Kiwi ACE program</t>
+    <t xml:space="preserve">Kiwi - Adolescents Coping with Emotions (Kiwi-ACE)</t>
   </si>
   <si>
     <t xml:space="preserve">0% AIAN, 0% Asian, 0% Black, 0% Latinx, 100% NHPI, 0% White, 0% Mixed, 0% Other</t>
@@ -1630,7 +1627,7 @@
     <t xml:space="preserve">2,664 students, 12 schools</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP-A; RAP-F</t>
+    <t xml:space="preserve">Resourceful Adolescent Program - Adolescents (RAP-A); Resourceful Adolescent Program - Family (RAP-F)</t>
   </si>
   <si>
     <t xml:space="preserve">https://psycnet.apa.org/record/2009-08717-006</t>
@@ -1943,7 +1940,7 @@
     <t xml:space="preserve">14.2 (0.65)</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP-Kiwi</t>
+    <t xml:space="preserve">Resourceful Adolescent Program-New Zealand version (RAP-Kiwi)</t>
   </si>
   <si>
     <t xml:space="preserve">Active: Placebo program</t>
@@ -1994,7 +1991,7 @@
     <t xml:space="preserve">13.58 (0.61)</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP Program</t>
+    <t xml:space="preserve">Resourceful Adolescent Program (RAP)</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.sciencedirect.com/science/article/abs/pii/S0022440504000676</t>
@@ -2173,7 +2170,7 @@
     <t xml:space="preserve">10.44 (0.69)</t>
   </si>
   <si>
-    <t xml:space="preserve">Normal Penn group; Reversed Penn Group</t>
+    <t xml:space="preserve">Penn Prevention Program</t>
   </si>
   <si>
     <t xml:space="preserve">https://psycnet.apa.org/record/2002-10530-003</t>
@@ -2222,9 +2219,6 @@
     <t xml:space="preserve">13.49 (0.54)</t>
   </si>
   <si>
-    <t xml:space="preserve">RAP–A; RAP-F</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cluster (Not reported)</t>
   </si>
   <si>
@@ -2409,9 +2403,6 @@
   </si>
   <si>
     <t xml:space="preserve">15.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preventive Health Class</t>
   </si>
 </sst>
 </file>
@@ -4370,10 +4361,10 @@
         <v>33</v>
       </c>
       <c r="L21" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" t="s">
         <v>283</v>
-      </c>
-      <c r="M21" t="s">
-        <v>284</v>
       </c>
       <c r="N21" t="s">
         <v>145</v>
@@ -4397,7 +4388,7 @@
         <v>33</v>
       </c>
       <c r="U21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V21" t="s">
         <v>92</v>
@@ -4406,27 +4397,27 @@
         <v>205</v>
       </c>
       <c r="X21" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y21" t="s">
         <v>286</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>287</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>288</v>
+      </c>
+      <c r="B22" t="s">
         <v>289</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>290</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>291</v>
-      </c>
-      <c r="D22" t="s">
-        <v>292</v>
       </c>
       <c r="E22" t="s">
         <v>52</v>
@@ -4441,16 +4432,16 @@
         <v>71</v>
       </c>
       <c r="I22" t="s">
+        <v>292</v>
+      </c>
+      <c r="J22" t="s">
         <v>293</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>294</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>295</v>
-      </c>
-      <c r="L22" t="s">
-        <v>296</v>
       </c>
       <c r="M22" t="s">
         <v>59</v>
@@ -4465,19 +4456,19 @@
         <v>60</v>
       </c>
       <c r="Q22" t="s">
+        <v>296</v>
+      </c>
+      <c r="R22" t="s">
+        <v>33</v>
+      </c>
+      <c r="S22" t="s">
+        <v>33</v>
+      </c>
+      <c r="T22" t="s">
+        <v>33</v>
+      </c>
+      <c r="U22" t="s">
         <v>297</v>
-      </c>
-      <c r="R22" t="s">
-        <v>33</v>
-      </c>
-      <c r="S22" t="s">
-        <v>33</v>
-      </c>
-      <c r="T22" t="s">
-        <v>33</v>
-      </c>
-      <c r="U22" t="s">
-        <v>298</v>
       </c>
       <c r="V22" t="s">
         <v>122</v>
@@ -4489,7 +4480,7 @@
         <v>46</v>
       </c>
       <c r="Y22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Z22" t="s">
         <v>228</v>
@@ -4497,40 +4488,40 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>299</v>
+      </c>
+      <c r="B23" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" t="s">
         <v>300</v>
       </c>
-      <c r="B23" t="s">
-        <v>290</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>301</v>
-      </c>
-      <c r="D23" t="s">
-        <v>302</v>
       </c>
       <c r="E23" t="s">
         <v>232</v>
       </c>
       <c r="F23" t="s">
+        <v>302</v>
+      </c>
+      <c r="G23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" t="s">
         <v>303</v>
       </c>
-      <c r="G23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>304</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>305</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>306</v>
-      </c>
-      <c r="L23" t="s">
-        <v>307</v>
       </c>
       <c r="M23" t="s">
         <v>59</v>
@@ -4569,22 +4560,22 @@
         <v>46</v>
       </c>
       <c r="Y23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Z23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>308</v>
+      </c>
+      <c r="B24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" t="s">
         <v>309</v>
       </c>
-      <c r="B24" t="s">
-        <v>290</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>310</v>
-      </c>
-      <c r="D24" t="s">
-        <v>311</v>
       </c>
       <c r="E24" t="s">
         <v>186</v>
@@ -4599,16 +4590,16 @@
         <v>33</v>
       </c>
       <c r="I24" t="s">
+        <v>311</v>
+      </c>
+      <c r="J24" t="s">
         <v>312</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>313</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>314</v>
-      </c>
-      <c r="L24" t="s">
-        <v>315</v>
       </c>
       <c r="M24" t="s">
         <v>259</v>
@@ -4635,7 +4626,7 @@
         <v>33</v>
       </c>
       <c r="U24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V24" t="s">
         <v>92</v>
@@ -4647,30 +4638,30 @@
         <v>46</v>
       </c>
       <c r="Y24" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z24" t="s">
         <v>317</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>318</v>
+      </c>
+      <c r="B25" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" t="s">
         <v>319</v>
       </c>
-      <c r="B25" t="s">
-        <v>290</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>320</v>
-      </c>
-      <c r="D25" t="s">
-        <v>321</v>
       </c>
       <c r="E25" t="s">
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G25" t="s">
         <v>33</v>
@@ -4679,19 +4670,19 @@
         <v>269</v>
       </c>
       <c r="I25" t="s">
+        <v>322</v>
+      </c>
+      <c r="J25" t="s">
         <v>323</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>324</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>325</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>326</v>
-      </c>
-      <c r="M25" t="s">
-        <v>327</v>
       </c>
       <c r="N25" t="s">
         <v>89</v>
@@ -4703,10 +4694,10 @@
         <v>41</v>
       </c>
       <c r="Q25" t="s">
+        <v>327</v>
+      </c>
+      <c r="R25" t="s">
         <v>328</v>
-      </c>
-      <c r="R25" t="s">
-        <v>329</v>
       </c>
       <c r="S25" t="s">
         <v>33</v>
@@ -4727,30 +4718,30 @@
         <v>46</v>
       </c>
       <c r="Y25" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z25" t="s">
         <v>330</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>331</v>
+      </c>
+      <c r="B26" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" t="s">
         <v>332</v>
       </c>
-      <c r="B26" t="s">
-        <v>290</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>333</v>
-      </c>
-      <c r="D26" t="s">
-        <v>334</v>
       </c>
       <c r="E26" t="s">
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G26" t="s">
         <v>33</v>
@@ -4759,22 +4750,22 @@
         <v>269</v>
       </c>
       <c r="I26" t="s">
+        <v>335</v>
+      </c>
+      <c r="J26" t="s">
         <v>336</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" t="s">
         <v>337</v>
-      </c>
-      <c r="K26" t="s">
-        <v>33</v>
-      </c>
-      <c r="L26" t="s">
-        <v>338</v>
       </c>
       <c r="M26" t="s">
         <v>259</v>
       </c>
       <c r="N26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O26" t="s">
         <v>40</v>
@@ -4783,7 +4774,7 @@
         <v>60</v>
       </c>
       <c r="Q26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R26" t="s">
         <v>33</v>
@@ -4807,33 +4798,33 @@
         <v>46</v>
       </c>
       <c r="Y26" t="s">
+        <v>340</v>
+      </c>
+      <c r="Z26" t="s">
         <v>341</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>342</v>
+      </c>
+      <c r="B27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C27" t="s">
         <v>343</v>
       </c>
-      <c r="B27" t="s">
-        <v>290</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>344</v>
-      </c>
-      <c r="D27" t="s">
-        <v>345</v>
       </c>
       <c r="E27" t="s">
         <v>98</v>
       </c>
       <c r="F27" t="s">
+        <v>345</v>
+      </c>
+      <c r="G27" t="s">
         <v>346</v>
-      </c>
-      <c r="G27" t="s">
-        <v>347</v>
       </c>
       <c r="H27" t="s">
         <v>33</v>
@@ -4842,13 +4833,13 @@
         <v>72</v>
       </c>
       <c r="J27" t="s">
+        <v>347</v>
+      </c>
+      <c r="K27" t="s">
         <v>348</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>349</v>
-      </c>
-      <c r="L27" t="s">
-        <v>350</v>
       </c>
       <c r="M27" t="s">
         <v>59</v>
@@ -4857,7 +4848,7 @@
         <v>39</v>
       </c>
       <c r="O27" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P27" t="s">
         <v>41</v>
@@ -4866,13 +4857,13 @@
         <v>90</v>
       </c>
       <c r="R27" t="s">
+        <v>351</v>
+      </c>
+      <c r="S27" t="s">
+        <v>33</v>
+      </c>
+      <c r="T27" t="s">
         <v>352</v>
-      </c>
-      <c r="S27" t="s">
-        <v>33</v>
-      </c>
-      <c r="T27" t="s">
-        <v>353</v>
       </c>
       <c r="U27" t="s">
         <v>33</v>
@@ -4887,27 +4878,27 @@
         <v>46</v>
       </c>
       <c r="Y27" t="s">
+        <v>353</v>
+      </c>
+      <c r="Z27" t="s">
         <v>354</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" t="s">
         <v>356</v>
       </c>
-      <c r="B28" t="s">
-        <v>290</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>357</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>358</v>
-      </c>
-      <c r="E28" t="s">
-        <v>359</v>
       </c>
       <c r="F28" t="s">
         <v>53</v>
@@ -4919,25 +4910,25 @@
         <v>33</v>
       </c>
       <c r="I28" t="s">
+        <v>359</v>
+      </c>
+      <c r="J28" t="s">
         <v>360</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>361</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>362</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>363</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>364</v>
       </c>
-      <c r="N28" t="s">
-        <v>365</v>
-      </c>
       <c r="O28" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P28" t="s">
         <v>60</v>
@@ -4955,40 +4946,40 @@
         <v>33</v>
       </c>
       <c r="U28" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V28" t="s">
         <v>45</v>
       </c>
       <c r="W28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="X28" t="s">
         <v>46</v>
       </c>
       <c r="Y28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Z28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>366</v>
+      </c>
+      <c r="B29" t="s">
         <v>367</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>368</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>369</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>370</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>371</v>
-      </c>
-      <c r="F29" t="s">
-        <v>372</v>
       </c>
       <c r="G29" t="s">
         <v>32</v>
@@ -5000,16 +4991,16 @@
         <v>270</v>
       </c>
       <c r="J29" t="s">
+        <v>372</v>
+      </c>
+      <c r="K29" t="s">
         <v>373</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>374</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>375</v>
-      </c>
-      <c r="M29" t="s">
-        <v>376</v>
       </c>
       <c r="N29" t="s">
         <v>89</v>
@@ -5021,10 +5012,10 @@
         <v>77</v>
       </c>
       <c r="Q29" t="s">
+        <v>376</v>
+      </c>
+      <c r="R29" t="s">
         <v>377</v>
-      </c>
-      <c r="R29" t="s">
-        <v>378</v>
       </c>
       <c r="S29" t="s">
         <v>33</v>
@@ -5042,30 +5033,30 @@
         <v>205</v>
       </c>
       <c r="X29" t="s">
+        <v>378</v>
+      </c>
+      <c r="Y29" t="s">
         <v>379</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>380</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>381</v>
+      </c>
+      <c r="B30" t="s">
+        <v>367</v>
+      </c>
+      <c r="C30" t="s">
         <v>382</v>
       </c>
-      <c r="B30" t="s">
-        <v>368</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>383</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>384</v>
-      </c>
-      <c r="E30" t="s">
-        <v>385</v>
       </c>
       <c r="F30" t="s">
         <v>53</v>
@@ -5077,16 +5068,16 @@
         <v>269</v>
       </c>
       <c r="I30" t="s">
+        <v>385</v>
+      </c>
+      <c r="J30" t="s">
         <v>386</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" t="s">
         <v>387</v>
-      </c>
-      <c r="K30" t="s">
-        <v>33</v>
-      </c>
-      <c r="L30" t="s">
-        <v>388</v>
       </c>
       <c r="M30" t="s">
         <v>59</v>
@@ -5113,7 +5104,7 @@
         <v>33</v>
       </c>
       <c r="U30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="V30" t="s">
         <v>274</v>
@@ -5122,33 +5113,33 @@
         <v>205</v>
       </c>
       <c r="X30" t="s">
+        <v>389</v>
+      </c>
+      <c r="Y30" t="s">
         <v>390</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>391</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>392</v>
+      </c>
+      <c r="B31" t="s">
+        <v>367</v>
+      </c>
+      <c r="C31" t="s">
         <v>393</v>
       </c>
-      <c r="B31" t="s">
-        <v>368</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>394</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>395</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>396</v>
-      </c>
-      <c r="F31" t="s">
-        <v>397</v>
       </c>
       <c r="G31" t="s">
         <v>32</v>
@@ -5157,16 +5148,16 @@
         <v>71</v>
       </c>
       <c r="I31" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J31" t="s">
+        <v>397</v>
+      </c>
+      <c r="K31" t="s">
         <v>398</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>399</v>
-      </c>
-      <c r="L31" t="s">
-        <v>400</v>
       </c>
       <c r="M31" t="s">
         <v>59</v>
@@ -5181,7 +5172,7 @@
         <v>60</v>
       </c>
       <c r="Q31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R31" t="s">
         <v>33</v>
@@ -5193,36 +5184,36 @@
         <v>33</v>
       </c>
       <c r="U31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V31" t="s">
         <v>45</v>
       </c>
       <c r="W31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="X31" t="s">
         <v>46</v>
       </c>
       <c r="Y31" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z31" t="s">
         <v>401</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>402</v>
+      </c>
+      <c r="B32" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" t="s">
         <v>403</v>
       </c>
-      <c r="B32" t="s">
-        <v>368</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>404</v>
-      </c>
-      <c r="D32" t="s">
-        <v>405</v>
       </c>
       <c r="E32" t="s">
         <v>267</v>
@@ -5240,16 +5231,16 @@
         <v>281</v>
       </c>
       <c r="J32" t="s">
+        <v>405</v>
+      </c>
+      <c r="K32" t="s">
         <v>406</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>407</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>408</v>
-      </c>
-      <c r="M32" t="s">
-        <v>409</v>
       </c>
       <c r="N32" t="s">
         <v>89</v>
@@ -5261,19 +5252,19 @@
         <v>41</v>
       </c>
       <c r="Q32" t="s">
+        <v>409</v>
+      </c>
+      <c r="R32" t="s">
         <v>410</v>
       </c>
-      <c r="R32" t="s">
-        <v>411</v>
-      </c>
       <c r="S32" t="s">
         <v>33</v>
       </c>
       <c r="T32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="U32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V32" t="s">
         <v>92</v>
@@ -5285,54 +5276,54 @@
         <v>33</v>
       </c>
       <c r="Y32" t="s">
+        <v>411</v>
+      </c>
+      <c r="Z32" t="s">
         <v>412</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
+        <v>413</v>
+      </c>
+      <c r="B33" t="s">
+        <v>367</v>
+      </c>
+      <c r="C33" t="s">
         <v>414</v>
       </c>
-      <c r="B33" t="s">
-        <v>368</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>415</v>
-      </c>
-      <c r="D33" t="s">
-        <v>416</v>
       </c>
       <c r="E33" t="s">
         <v>98</v>
       </c>
       <c r="F33" t="s">
+        <v>416</v>
+      </c>
+      <c r="G33" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" t="s">
+        <v>33</v>
+      </c>
+      <c r="I33" t="s">
         <v>417</v>
       </c>
-      <c r="G33" t="s">
-        <v>33</v>
-      </c>
-      <c r="H33" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>418</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" t="s">
         <v>419</v>
       </c>
-      <c r="K33" t="s">
-        <v>33</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>420</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>421</v>
-      </c>
-      <c r="N33" t="s">
-        <v>422</v>
       </c>
       <c r="O33" t="s">
         <v>40</v>
@@ -5353,7 +5344,7 @@
         <v>33</v>
       </c>
       <c r="U33" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="V33" t="s">
         <v>45</v>
@@ -5365,54 +5356,54 @@
         <v>46</v>
       </c>
       <c r="Y33" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z33" t="s">
         <v>424</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B34" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C34" t="s">
+        <v>414</v>
+      </c>
+      <c r="D34" t="s">
         <v>415</v>
-      </c>
-      <c r="D34" t="s">
-        <v>416</v>
       </c>
       <c r="E34" t="s">
         <v>98</v>
       </c>
       <c r="F34" t="s">
+        <v>426</v>
+      </c>
+      <c r="G34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" t="s">
         <v>427</v>
       </c>
-      <c r="G34" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" t="s">
-        <v>33</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>428</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>429</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
+        <v>419</v>
+      </c>
+      <c r="M34" t="s">
+        <v>420</v>
+      </c>
+      <c r="N34" t="s">
         <v>430</v>
-      </c>
-      <c r="L34" t="s">
-        <v>420</v>
-      </c>
-      <c r="M34" t="s">
-        <v>421</v>
-      </c>
-      <c r="N34" t="s">
-        <v>431</v>
       </c>
       <c r="O34" t="s">
         <v>40</v>
@@ -5424,16 +5415,16 @@
         <v>33</v>
       </c>
       <c r="R34" t="s">
+        <v>431</v>
+      </c>
+      <c r="S34" t="s">
+        <v>33</v>
+      </c>
+      <c r="T34" t="s">
         <v>432</v>
       </c>
-      <c r="S34" t="s">
-        <v>33</v>
-      </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>433</v>
-      </c>
-      <c r="U34" t="s">
-        <v>434</v>
       </c>
       <c r="V34" t="s">
         <v>45</v>
@@ -5445,30 +5436,30 @@
         <v>46</v>
       </c>
       <c r="Y34" t="s">
+        <v>423</v>
+      </c>
+      <c r="Z34" t="s">
         <v>424</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>434</v>
+      </c>
+      <c r="B35" t="s">
         <v>435</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>436</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>437</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>438</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>439</v>
-      </c>
-      <c r="F35" t="s">
-        <v>440</v>
       </c>
       <c r="G35" t="s">
         <v>33</v>
@@ -5480,22 +5471,22 @@
         <v>55</v>
       </c>
       <c r="J35" t="s">
+        <v>440</v>
+      </c>
+      <c r="K35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L35" t="s">
         <v>441</v>
-      </c>
-      <c r="K35" t="s">
-        <v>33</v>
-      </c>
-      <c r="L35" t="s">
-        <v>442</v>
       </c>
       <c r="M35" t="s">
         <v>38</v>
       </c>
       <c r="N35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O35" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P35" t="s">
         <v>77</v>
@@ -5519,36 +5510,36 @@
         <v>62</v>
       </c>
       <c r="W35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="X35" t="s">
         <v>46</v>
       </c>
       <c r="Y35" t="s">
+        <v>442</v>
+      </c>
+      <c r="Z35" t="s">
         <v>443</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>444</v>
+      </c>
+      <c r="B36" t="s">
         <v>445</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>446</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>447</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>370</v>
+      </c>
+      <c r="F36" t="s">
         <v>448</v>
-      </c>
-      <c r="E36" t="s">
-        <v>371</v>
-      </c>
-      <c r="F36" t="s">
-        <v>449</v>
       </c>
       <c r="G36" t="s">
         <v>32</v>
@@ -5557,16 +5548,16 @@
         <v>71</v>
       </c>
       <c r="I36" t="s">
+        <v>449</v>
+      </c>
+      <c r="J36" t="s">
         <v>450</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>451</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>452</v>
-      </c>
-      <c r="L36" t="s">
-        <v>453</v>
       </c>
       <c r="M36" t="s">
         <v>59</v>
@@ -5581,19 +5572,19 @@
         <v>77</v>
       </c>
       <c r="Q36" t="s">
+        <v>453</v>
+      </c>
+      <c r="R36" t="s">
         <v>454</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" t="s">
+        <v>33</v>
+      </c>
+      <c r="U36" t="s">
         <v>455</v>
-      </c>
-      <c r="S36" t="s">
-        <v>33</v>
-      </c>
-      <c r="T36" t="s">
-        <v>33</v>
-      </c>
-      <c r="U36" t="s">
-        <v>456</v>
       </c>
       <c r="V36" t="s">
         <v>274</v>
@@ -5602,30 +5593,30 @@
         <v>205</v>
       </c>
       <c r="X36" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Y36" t="s">
+        <v>456</v>
+      </c>
+      <c r="Z36" t="s">
         <v>457</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>458</v>
+      </c>
+      <c r="B37" t="s">
+        <v>445</v>
+      </c>
+      <c r="C37" t="s">
         <v>459</v>
       </c>
-      <c r="B37" t="s">
-        <v>446</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>460</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>461</v>
-      </c>
-      <c r="E37" t="s">
-        <v>462</v>
       </c>
       <c r="F37" t="s">
         <v>53</v>
@@ -5637,16 +5628,16 @@
         <v>71</v>
       </c>
       <c r="I37" t="s">
+        <v>462</v>
+      </c>
+      <c r="J37" t="s">
         <v>463</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" t="s">
         <v>464</v>
-      </c>
-      <c r="K37" t="s">
-        <v>33</v>
-      </c>
-      <c r="L37" t="s">
-        <v>465</v>
       </c>
       <c r="M37" t="s">
         <v>38</v>
@@ -5673,39 +5664,39 @@
         <v>33</v>
       </c>
       <c r="U37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="V37" t="s">
         <v>45</v>
       </c>
       <c r="W37" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="X37" t="s">
         <v>46</v>
       </c>
       <c r="Y37" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="Z37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>467</v>
+      </c>
+      <c r="B38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C38" t="s">
         <v>468</v>
       </c>
-      <c r="B38" t="s">
-        <v>446</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>469</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>470</v>
-      </c>
-      <c r="E38" t="s">
-        <v>471</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -5717,16 +5708,16 @@
         <v>33</v>
       </c>
       <c r="I38" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J38" t="s">
+        <v>471</v>
+      </c>
+      <c r="K38" t="s">
         <v>472</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>473</v>
-      </c>
-      <c r="L38" t="s">
-        <v>474</v>
       </c>
       <c r="M38" t="s">
         <v>259</v>
@@ -5744,7 +5735,7 @@
         <v>33</v>
       </c>
       <c r="R38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="S38" t="s">
         <v>33</v>
@@ -5753,40 +5744,40 @@
         <v>33</v>
       </c>
       <c r="U38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V38" t="s">
         <v>45</v>
       </c>
       <c r="W38" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="X38" t="s">
         <v>46</v>
       </c>
       <c r="Y38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="Z38"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>476</v>
+      </c>
+      <c r="B39" t="s">
         <v>477</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>478</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>479</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>480</v>
       </c>
-      <c r="E39" t="s">
-        <v>481</v>
-      </c>
       <c r="F39" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G39" t="s">
         <v>70</v>
@@ -5795,19 +5786,19 @@
         <v>71</v>
       </c>
       <c r="I39" t="s">
+        <v>481</v>
+      </c>
+      <c r="J39" t="s">
         <v>482</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>483</v>
       </c>
-      <c r="K39" t="s">
-        <v>484</v>
-      </c>
       <c r="L39" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N39" t="s">
         <v>89</v>
@@ -5819,52 +5810,52 @@
         <v>77</v>
       </c>
       <c r="Q39" t="s">
+        <v>484</v>
+      </c>
+      <c r="R39" t="s">
+        <v>33</v>
+      </c>
+      <c r="S39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T39" t="s">
         <v>485</v>
       </c>
-      <c r="R39" t="s">
-        <v>33</v>
-      </c>
-      <c r="S39" t="s">
-        <v>33</v>
-      </c>
-      <c r="T39" t="s">
+      <c r="U39" t="s">
+        <v>388</v>
+      </c>
+      <c r="V39" t="s">
         <v>486</v>
-      </c>
-      <c r="U39" t="s">
-        <v>389</v>
-      </c>
-      <c r="V39" t="s">
-        <v>487</v>
       </c>
       <c r="W39" t="s">
         <v>205</v>
       </c>
       <c r="X39" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y39" t="s">
         <v>488</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>489</v>
       </c>
       <c r="Z39"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>489</v>
+      </c>
+      <c r="B40" t="s">
+        <v>477</v>
+      </c>
+      <c r="C40" t="s">
         <v>490</v>
       </c>
-      <c r="B40" t="s">
-        <v>478</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>491</v>
-      </c>
-      <c r="D40" t="s">
-        <v>492</v>
       </c>
       <c r="E40" t="s">
         <v>52</v>
       </c>
       <c r="F40" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G40" t="s">
         <v>33</v>
@@ -5873,16 +5864,16 @@
         <v>71</v>
       </c>
       <c r="I40" t="s">
+        <v>493</v>
+      </c>
+      <c r="J40" t="s">
         <v>494</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>495</v>
       </c>
-      <c r="K40" t="s">
-        <v>496</v>
-      </c>
       <c r="L40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M40" t="s">
         <v>59</v>
@@ -5909,7 +5900,7 @@
         <v>33</v>
       </c>
       <c r="U40" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V40" t="s">
         <v>62</v>
@@ -5921,28 +5912,28 @@
         <v>46</v>
       </c>
       <c r="Y40" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Z40"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>497</v>
+      </c>
+      <c r="B41" t="s">
+        <v>477</v>
+      </c>
+      <c r="C41" t="s">
         <v>498</v>
       </c>
-      <c r="B41" t="s">
-        <v>478</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>499</v>
-      </c>
-      <c r="D41" t="s">
-        <v>500</v>
       </c>
       <c r="E41" t="s">
         <v>52</v>
       </c>
       <c r="F41" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G41" t="s">
         <v>32</v>
@@ -5954,13 +5945,13 @@
         <v>84</v>
       </c>
       <c r="J41" t="s">
+        <v>501</v>
+      </c>
+      <c r="K41" t="s">
         <v>502</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>503</v>
-      </c>
-      <c r="L41" t="s">
-        <v>504</v>
       </c>
       <c r="M41" t="s">
         <v>177</v>
@@ -5975,13 +5966,13 @@
         <v>60</v>
       </c>
       <c r="Q41" t="s">
+        <v>504</v>
+      </c>
+      <c r="R41" t="s">
+        <v>33</v>
+      </c>
+      <c r="S41" t="s">
         <v>505</v>
-      </c>
-      <c r="R41" t="s">
-        <v>33</v>
-      </c>
-      <c r="S41" t="s">
-        <v>506</v>
       </c>
       <c r="T41" t="s">
         <v>33</v>
@@ -5999,30 +5990,30 @@
         <v>46</v>
       </c>
       <c r="Y41" t="s">
+        <v>506</v>
+      </c>
+      <c r="Z41" t="s">
         <v>507</v>
-      </c>
-      <c r="Z41" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>508</v>
+      </c>
+      <c r="B42" t="s">
         <v>509</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>510</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>511</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>512</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>513</v>
-      </c>
-      <c r="F42" t="s">
-        <v>514</v>
       </c>
       <c r="G42" t="s">
         <v>33</v>
@@ -6034,19 +6025,19 @@
         <v>281</v>
       </c>
       <c r="J42" t="s">
+        <v>514</v>
+      </c>
+      <c r="K42" t="s">
         <v>515</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>516</v>
-      </c>
-      <c r="L42" t="s">
-        <v>517</v>
       </c>
       <c r="M42" t="s">
         <v>259</v>
       </c>
       <c r="N42" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O42" t="s">
         <v>40</v>
@@ -6067,60 +6058,60 @@
         <v>33</v>
       </c>
       <c r="U42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V42" t="s">
         <v>92</v>
       </c>
       <c r="W42" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="X42" t="s">
         <v>46</v>
       </c>
       <c r="Y42" t="s">
+        <v>517</v>
+      </c>
+      <c r="Z42" t="s">
         <v>518</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>519</v>
+      </c>
+      <c r="B43" t="s">
+        <v>509</v>
+      </c>
+      <c r="C43" t="s">
         <v>520</v>
       </c>
-      <c r="B43" t="s">
-        <v>510</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>521</v>
-      </c>
-      <c r="D43" t="s">
-        <v>522</v>
       </c>
       <c r="E43" t="s">
         <v>52</v>
       </c>
       <c r="F43" t="s">
+        <v>522</v>
+      </c>
+      <c r="G43" t="s">
         <v>523</v>
-      </c>
-      <c r="G43" t="s">
-        <v>524</v>
       </c>
       <c r="H43" t="s">
         <v>163</v>
       </c>
       <c r="I43" t="s">
+        <v>524</v>
+      </c>
+      <c r="J43" t="s">
         <v>525</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>526</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>527</v>
-      </c>
-      <c r="L43" t="s">
-        <v>528</v>
       </c>
       <c r="M43" t="s">
         <v>38</v>
@@ -6135,19 +6126,19 @@
         <v>60</v>
       </c>
       <c r="Q43" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="R43" t="s">
         <v>33</v>
       </c>
       <c r="S43" t="s">
+        <v>528</v>
+      </c>
+      <c r="T43" t="s">
+        <v>33</v>
+      </c>
+      <c r="U43" t="s">
         <v>529</v>
-      </c>
-      <c r="T43" t="s">
-        <v>33</v>
-      </c>
-      <c r="U43" t="s">
-        <v>530</v>
       </c>
       <c r="V43" t="s">
         <v>45</v>
@@ -6159,24 +6150,24 @@
         <v>46</v>
       </c>
       <c r="Y43" t="s">
+        <v>530</v>
+      </c>
+      <c r="Z43" t="s">
         <v>531</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>532</v>
+      </c>
+      <c r="B44" t="s">
+        <v>509</v>
+      </c>
+      <c r="C44" t="s">
         <v>533</v>
       </c>
-      <c r="B44" t="s">
-        <v>510</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>534</v>
-      </c>
-      <c r="D44" t="s">
-        <v>535</v>
       </c>
       <c r="E44" t="s">
         <v>52</v>
@@ -6191,16 +6182,16 @@
         <v>33</v>
       </c>
       <c r="I44" t="s">
+        <v>535</v>
+      </c>
+      <c r="J44" t="s">
         <v>536</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L44" t="s">
         <v>537</v>
-      </c>
-      <c r="K44" t="s">
-        <v>33</v>
-      </c>
-      <c r="L44" t="s">
-        <v>538</v>
       </c>
       <c r="M44" t="s">
         <v>259</v>
@@ -6227,7 +6218,7 @@
         <v>33</v>
       </c>
       <c r="U44" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V44" t="s">
         <v>33</v>
@@ -6239,24 +6230,24 @@
         <v>46</v>
       </c>
       <c r="Y44" t="s">
+        <v>538</v>
+      </c>
+      <c r="Z44" t="s">
         <v>539</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>540</v>
+      </c>
+      <c r="B45" t="s">
+        <v>509</v>
+      </c>
+      <c r="C45" t="s">
         <v>541</v>
       </c>
-      <c r="B45" t="s">
-        <v>510</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>542</v>
-      </c>
-      <c r="D45" t="s">
-        <v>543</v>
       </c>
       <c r="E45" t="s">
         <v>52</v>
@@ -6271,16 +6262,16 @@
         <v>33</v>
       </c>
       <c r="I45" t="s">
+        <v>543</v>
+      </c>
+      <c r="J45" t="s">
         <v>544</v>
       </c>
-      <c r="J45" t="s">
-        <v>545</v>
-      </c>
       <c r="K45" t="s">
         <v>33</v>
       </c>
       <c r="L45" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M45" t="s">
         <v>59</v>
@@ -6289,7 +6280,7 @@
         <v>145</v>
       </c>
       <c r="O45" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P45" t="s">
         <v>77</v>
@@ -6307,7 +6298,7 @@
         <v>33</v>
       </c>
       <c r="U45" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V45" t="s">
         <v>92</v>
@@ -6319,27 +6310,27 @@
         <v>46</v>
       </c>
       <c r="Y45" t="s">
+        <v>546</v>
+      </c>
+      <c r="Z45" t="s">
         <v>547</v>
-      </c>
-      <c r="Z45" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>548</v>
+      </c>
+      <c r="B46" t="s">
         <v>549</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>550</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>404</v>
+      </c>
+      <c r="E46" t="s">
         <v>551</v>
-      </c>
-      <c r="D46" t="s">
-        <v>405</v>
-      </c>
-      <c r="E46" t="s">
-        <v>552</v>
       </c>
       <c r="F46" t="s">
         <v>53</v>
@@ -6351,16 +6342,16 @@
         <v>33</v>
       </c>
       <c r="I46" t="s">
+        <v>552</v>
+      </c>
+      <c r="J46" t="s">
         <v>553</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>554</v>
       </c>
-      <c r="K46" t="s">
-        <v>555</v>
-      </c>
       <c r="L46" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M46" t="s">
         <v>59</v>
@@ -6375,7 +6366,7 @@
         <v>41</v>
       </c>
       <c r="Q46" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="R46" t="s">
         <v>33</v>
@@ -6393,36 +6384,36 @@
         <v>274</v>
       </c>
       <c r="W46" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="X46" t="s">
         <v>46</v>
       </c>
       <c r="Y46" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="Z46" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>557</v>
+      </c>
+      <c r="B47" t="s">
         <v>558</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>559</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>560</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>480</v>
+      </c>
+      <c r="F47" t="s">
         <v>561</v>
-      </c>
-      <c r="E47" t="s">
-        <v>481</v>
-      </c>
-      <c r="F47" t="s">
-        <v>562</v>
       </c>
       <c r="G47" t="s">
         <v>32</v>
@@ -6431,16 +6422,16 @@
         <v>33</v>
       </c>
       <c r="I47" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J47" t="s">
+        <v>562</v>
+      </c>
+      <c r="K47" t="s">
         <v>563</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>564</v>
-      </c>
-      <c r="L47" t="s">
-        <v>565</v>
       </c>
       <c r="M47" t="s">
         <v>259</v>
@@ -6455,7 +6446,7 @@
         <v>77</v>
       </c>
       <c r="Q47" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="R47" t="s">
         <v>43</v>
@@ -6467,7 +6458,7 @@
         <v>33</v>
       </c>
       <c r="U47" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="V47" t="s">
         <v>274</v>
@@ -6476,33 +6467,33 @@
         <v>205</v>
       </c>
       <c r="X47" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Y47" t="s">
+        <v>565</v>
+      </c>
+      <c r="Z47" t="s">
         <v>566</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B48" t="s">
+        <v>558</v>
+      </c>
+      <c r="C48" t="s">
         <v>559</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>560</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
+        <v>480</v>
+      </c>
+      <c r="F48" t="s">
         <v>561</v>
-      </c>
-      <c r="E48" t="s">
-        <v>481</v>
-      </c>
-      <c r="F48" t="s">
-        <v>562</v>
       </c>
       <c r="G48" t="s">
         <v>32</v>
@@ -6511,16 +6502,16 @@
         <v>33</v>
       </c>
       <c r="I48" t="s">
+        <v>568</v>
+      </c>
+      <c r="J48" t="s">
         <v>569</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>570</v>
       </c>
-      <c r="K48" t="s">
-        <v>571</v>
-      </c>
       <c r="L48" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M48" t="s">
         <v>259</v>
@@ -6535,19 +6526,19 @@
         <v>77</v>
       </c>
       <c r="Q48" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="R48" t="s">
+        <v>571</v>
+      </c>
+      <c r="S48" t="s">
+        <v>33</v>
+      </c>
+      <c r="T48" t="s">
+        <v>33</v>
+      </c>
+      <c r="U48" t="s">
         <v>572</v>
-      </c>
-      <c r="S48" t="s">
-        <v>33</v>
-      </c>
-      <c r="T48" t="s">
-        <v>33</v>
-      </c>
-      <c r="U48" t="s">
-        <v>573</v>
       </c>
       <c r="V48" t="s">
         <v>274</v>
@@ -6556,33 +6547,33 @@
         <v>205</v>
       </c>
       <c r="X48" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Y48" t="s">
+        <v>565</v>
+      </c>
+      <c r="Z48" t="s">
         <v>566</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>573</v>
+      </c>
+      <c r="B49" t="s">
+        <v>558</v>
+      </c>
+      <c r="C49" t="s">
         <v>574</v>
       </c>
-      <c r="B49" t="s">
-        <v>559</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>575</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>576</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>577</v>
-      </c>
-      <c r="F49" t="s">
-        <v>578</v>
       </c>
       <c r="G49" t="s">
         <v>54</v>
@@ -6591,16 +6582,16 @@
         <v>33</v>
       </c>
       <c r="I49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J49" t="s">
+        <v>578</v>
+      </c>
+      <c r="K49" t="s">
         <v>579</v>
       </c>
-      <c r="K49" t="s">
+      <c r="L49" t="s">
         <v>580</v>
-      </c>
-      <c r="L49" t="s">
-        <v>581</v>
       </c>
       <c r="M49" t="s">
         <v>59</v>
@@ -6618,7 +6609,7 @@
         <v>42</v>
       </c>
       <c r="R49" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="S49" t="s">
         <v>33</v>
@@ -6627,7 +6618,7 @@
         <v>33</v>
       </c>
       <c r="U49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="V49" t="s">
         <v>92</v>
@@ -6636,27 +6627,27 @@
         <v>205</v>
       </c>
       <c r="X49" t="s">
+        <v>582</v>
+      </c>
+      <c r="Y49" t="s">
         <v>583</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>584</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>585</v>
+      </c>
+      <c r="B50" t="s">
         <v>586</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>587</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>588</v>
-      </c>
-      <c r="D50" t="s">
-        <v>589</v>
       </c>
       <c r="E50" t="s">
         <v>52</v>
@@ -6674,13 +6665,13 @@
         <v>55</v>
       </c>
       <c r="J50" t="s">
+        <v>589</v>
+      </c>
+      <c r="K50" t="s">
         <v>590</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>591</v>
-      </c>
-      <c r="L50" t="s">
-        <v>592</v>
       </c>
       <c r="M50" t="s">
         <v>59</v>
@@ -6695,7 +6686,7 @@
         <v>77</v>
       </c>
       <c r="Q50" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="R50" t="s">
         <v>33</v>
@@ -6719,7 +6710,7 @@
         <v>46</v>
       </c>
       <c r="Y50" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="Z50" t="s">
         <v>228</v>
@@ -6727,46 +6718,46 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>594</v>
+      </c>
+      <c r="B51" t="s">
+        <v>586</v>
+      </c>
+      <c r="C51" t="s">
         <v>595</v>
       </c>
-      <c r="B51" t="s">
-        <v>587</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>596</v>
-      </c>
-      <c r="D51" t="s">
-        <v>597</v>
       </c>
       <c r="E51" t="s">
         <v>52</v>
       </c>
       <c r="F51" t="s">
+        <v>597</v>
+      </c>
+      <c r="G51" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" t="s">
+        <v>33</v>
+      </c>
+      <c r="I51" t="s">
+        <v>359</v>
+      </c>
+      <c r="J51" t="s">
         <v>598</v>
       </c>
-      <c r="G51" t="s">
-        <v>33</v>
-      </c>
-      <c r="H51" t="s">
-        <v>33</v>
-      </c>
-      <c r="I51" t="s">
-        <v>360</v>
-      </c>
-      <c r="J51" t="s">
-        <v>599</v>
-      </c>
       <c r="K51" t="s">
         <v>33</v>
       </c>
       <c r="L51" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M51" t="s">
         <v>59</v>
       </c>
       <c r="N51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="O51" t="s">
         <v>40</v>
@@ -6787,7 +6778,7 @@
         <v>33</v>
       </c>
       <c r="U51" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V51" t="s">
         <v>45</v>
@@ -6799,24 +6790,24 @@
         <v>46</v>
       </c>
       <c r="Y51" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="Z51" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>601</v>
+      </c>
+      <c r="B52" t="s">
+        <v>586</v>
+      </c>
+      <c r="C52" t="s">
         <v>602</v>
       </c>
-      <c r="B52" t="s">
-        <v>587</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>603</v>
-      </c>
-      <c r="D52" t="s">
-        <v>604</v>
       </c>
       <c r="E52" t="s">
         <v>52</v>
@@ -6825,22 +6816,22 @@
         <v>53</v>
       </c>
       <c r="G52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H52" t="s">
+        <v>604</v>
+      </c>
+      <c r="I52" t="s">
         <v>605</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>606</v>
       </c>
-      <c r="J52" t="s">
+      <c r="K52" t="s">
         <v>607</v>
       </c>
-      <c r="K52" t="s">
+      <c r="L52" t="s">
         <v>608</v>
-      </c>
-      <c r="L52" t="s">
-        <v>609</v>
       </c>
       <c r="M52" t="s">
         <v>259</v>
@@ -6867,7 +6858,7 @@
         <v>33</v>
       </c>
       <c r="U52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V52" t="s">
         <v>33</v>
@@ -6879,24 +6870,24 @@
         <v>46</v>
       </c>
       <c r="Y52" t="s">
+        <v>609</v>
+      </c>
+      <c r="Z52" t="s">
         <v>610</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>611</v>
+      </c>
+      <c r="B53" t="s">
         <v>612</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>613</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>614</v>
-      </c>
-      <c r="D53" t="s">
-        <v>615</v>
       </c>
       <c r="E53" t="s">
         <v>267</v>
@@ -6908,19 +6899,19 @@
         <v>33</v>
       </c>
       <c r="H53" t="s">
+        <v>615</v>
+      </c>
+      <c r="I53" t="s">
         <v>616</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>617</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>618</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>619</v>
-      </c>
-      <c r="L53" t="s">
-        <v>620</v>
       </c>
       <c r="M53" t="s">
         <v>259</v>
@@ -6938,16 +6929,16 @@
         <v>237</v>
       </c>
       <c r="R53" t="s">
+        <v>620</v>
+      </c>
+      <c r="S53" t="s">
+        <v>33</v>
+      </c>
+      <c r="T53" t="s">
+        <v>33</v>
+      </c>
+      <c r="U53" t="s">
         <v>621</v>
-      </c>
-      <c r="S53" t="s">
-        <v>33</v>
-      </c>
-      <c r="T53" t="s">
-        <v>33</v>
-      </c>
-      <c r="U53" t="s">
-        <v>622</v>
       </c>
       <c r="V53" t="s">
         <v>33</v>
@@ -6959,48 +6950,48 @@
         <v>33</v>
       </c>
       <c r="Y53" t="s">
+        <v>622</v>
+      </c>
+      <c r="Z53" t="s">
         <v>623</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>624</v>
+      </c>
+      <c r="B54" t="s">
+        <v>612</v>
+      </c>
+      <c r="C54" t="s">
         <v>625</v>
       </c>
-      <c r="B54" t="s">
-        <v>613</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>626</v>
-      </c>
-      <c r="D54" t="s">
-        <v>627</v>
       </c>
       <c r="E54" t="s">
         <v>52</v>
       </c>
       <c r="F54" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G54" t="s">
         <v>33</v>
       </c>
       <c r="H54" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I54" t="s">
         <v>281</v>
       </c>
       <c r="J54" t="s">
+        <v>628</v>
+      </c>
+      <c r="K54" t="s">
         <v>629</v>
       </c>
-      <c r="K54" t="s">
+      <c r="L54" t="s">
         <v>630</v>
-      </c>
-      <c r="L54" t="s">
-        <v>631</v>
       </c>
       <c r="M54" t="s">
         <v>38</v>
@@ -7015,7 +7006,7 @@
         <v>60</v>
       </c>
       <c r="Q54" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="R54" t="s">
         <v>33</v>
@@ -7027,7 +7018,7 @@
         <v>33</v>
       </c>
       <c r="U54" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V54" t="s">
         <v>92</v>
@@ -7039,49 +7030,49 @@
         <v>46</v>
       </c>
       <c r="Y54" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="Z54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>633</v>
+      </c>
+      <c r="B55" t="s">
         <v>634</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>635</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>636</v>
       </c>
-      <c r="D55" t="s">
-        <v>637</v>
-      </c>
       <c r="E55" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F55" t="s">
         <v>53</v>
       </c>
       <c r="G55" t="s">
+        <v>637</v>
+      </c>
+      <c r="H55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I55" t="s">
         <v>638</v>
       </c>
-      <c r="H55" t="s">
-        <v>33</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>639</v>
       </c>
-      <c r="J55" t="s">
+      <c r="K55" t="s">
         <v>640</v>
       </c>
-      <c r="K55" t="s">
+      <c r="L55" t="s">
         <v>641</v>
       </c>
-      <c r="L55" t="s">
+      <c r="M55" t="s">
         <v>642</v>
-      </c>
-      <c r="M55" t="s">
-        <v>643</v>
       </c>
       <c r="N55" t="s">
         <v>89</v>
@@ -7096,7 +7087,7 @@
         <v>225</v>
       </c>
       <c r="R55" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="S55" t="s">
         <v>33</v>
@@ -7111,33 +7102,33 @@
         <v>33</v>
       </c>
       <c r="W55" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="X55" t="s">
         <v>46</v>
       </c>
       <c r="Y55" t="s">
+        <v>644</v>
+      </c>
+      <c r="Z55" t="s">
         <v>645</v>
-      </c>
-      <c r="Z55" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>646</v>
+      </c>
+      <c r="B56" t="s">
+        <v>634</v>
+      </c>
+      <c r="C56" t="s">
         <v>647</v>
       </c>
-      <c r="B56" t="s">
-        <v>635</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>648</v>
       </c>
-      <c r="D56" t="s">
-        <v>649</v>
-      </c>
       <c r="E56" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F56" t="s">
         <v>53</v>
@@ -7149,16 +7140,16 @@
         <v>33</v>
       </c>
       <c r="I56" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="J56" t="s">
+        <v>649</v>
+      </c>
+      <c r="K56" t="s">
+        <v>33</v>
+      </c>
+      <c r="L56" t="s">
         <v>650</v>
-      </c>
-      <c r="K56" t="s">
-        <v>33</v>
-      </c>
-      <c r="L56" t="s">
-        <v>651</v>
       </c>
       <c r="M56" t="s">
         <v>59</v>
@@ -7191,36 +7182,36 @@
         <v>274</v>
       </c>
       <c r="W56" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="X56" t="s">
         <v>46</v>
       </c>
       <c r="Y56" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="Z56" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>652</v>
+      </c>
+      <c r="B57" t="s">
+        <v>634</v>
+      </c>
+      <c r="C57" t="s">
         <v>653</v>
       </c>
-      <c r="B57" t="s">
-        <v>635</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>654</v>
-      </c>
-      <c r="D57" t="s">
-        <v>655</v>
       </c>
       <c r="E57" t="s">
         <v>52</v>
       </c>
       <c r="F57" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G57" t="s">
         <v>33</v>
@@ -7229,16 +7220,16 @@
         <v>269</v>
       </c>
       <c r="I57" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J57" t="s">
+        <v>656</v>
+      </c>
+      <c r="K57" t="s">
         <v>657</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>658</v>
-      </c>
-      <c r="L57" t="s">
-        <v>659</v>
       </c>
       <c r="M57" t="s">
         <v>259</v>
@@ -7247,7 +7238,7 @@
         <v>39</v>
       </c>
       <c r="O57" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P57" t="s">
         <v>60</v>
@@ -7265,7 +7256,7 @@
         <v>33</v>
       </c>
       <c r="U57" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V57" t="s">
         <v>45</v>
@@ -7277,27 +7268,27 @@
         <v>46</v>
       </c>
       <c r="Y57" t="s">
+        <v>659</v>
+      </c>
+      <c r="Z57" t="s">
         <v>660</v>
-      </c>
-      <c r="Z57" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>661</v>
+      </c>
+      <c r="B58" t="s">
         <v>662</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>663</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>664</v>
       </c>
-      <c r="D58" t="s">
-        <v>665</v>
-      </c>
       <c r="E58" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F58" t="s">
         <v>53</v>
@@ -7309,16 +7300,16 @@
         <v>33</v>
       </c>
       <c r="I58" t="s">
+        <v>665</v>
+      </c>
+      <c r="J58" t="s">
         <v>666</v>
       </c>
-      <c r="J58" t="s">
+      <c r="K58" t="s">
         <v>667</v>
       </c>
-      <c r="K58" t="s">
+      <c r="L58" t="s">
         <v>668</v>
-      </c>
-      <c r="L58" t="s">
-        <v>669</v>
       </c>
       <c r="M58" t="s">
         <v>59</v>
@@ -7333,10 +7324,10 @@
         <v>77</v>
       </c>
       <c r="Q58" t="s">
+        <v>669</v>
+      </c>
+      <c r="R58" t="s">
         <v>670</v>
-      </c>
-      <c r="R58" t="s">
-        <v>671</v>
       </c>
       <c r="S58" t="s">
         <v>33</v>
@@ -7354,27 +7345,27 @@
         <v>205</v>
       </c>
       <c r="X58" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Y58" t="s">
+        <v>671</v>
+      </c>
+      <c r="Z58" t="s">
         <v>672</v>
-      </c>
-      <c r="Z58" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>673</v>
+      </c>
+      <c r="B59" t="s">
+        <v>662</v>
+      </c>
+      <c r="C59" t="s">
         <v>674</v>
       </c>
-      <c r="B59" t="s">
-        <v>663</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>675</v>
-      </c>
-      <c r="D59" t="s">
-        <v>676</v>
       </c>
       <c r="E59" t="s">
         <v>52</v>
@@ -7389,16 +7380,16 @@
         <v>33</v>
       </c>
       <c r="I59" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J59" t="s">
+        <v>676</v>
+      </c>
+      <c r="K59" t="s">
         <v>677</v>
       </c>
-      <c r="K59" t="s">
+      <c r="L59" t="s">
         <v>678</v>
-      </c>
-      <c r="L59" t="s">
-        <v>679</v>
       </c>
       <c r="M59" t="s">
         <v>59</v>
@@ -7425,7 +7416,7 @@
         <v>33</v>
       </c>
       <c r="U59" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V59" t="s">
         <v>62</v>
@@ -7437,25 +7428,25 @@
         <v>46</v>
       </c>
       <c r="Y59" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="Z59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>680</v>
+      </c>
+      <c r="B60" t="s">
+        <v>662</v>
+      </c>
+      <c r="C60" t="s">
         <v>681</v>
       </c>
-      <c r="B60" t="s">
-        <v>663</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>682</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>683</v>
-      </c>
-      <c r="E60" t="s">
-        <v>684</v>
       </c>
       <c r="F60" t="s">
         <v>53</v>
@@ -7467,16 +7458,16 @@
         <v>71</v>
       </c>
       <c r="I60" t="s">
+        <v>684</v>
+      </c>
+      <c r="J60" t="s">
         <v>685</v>
       </c>
-      <c r="J60" t="s">
+      <c r="K60" t="s">
         <v>686</v>
       </c>
-      <c r="K60" t="s">
+      <c r="L60" t="s">
         <v>687</v>
-      </c>
-      <c r="L60" t="s">
-        <v>688</v>
       </c>
       <c r="M60" t="s">
         <v>259</v>
@@ -7491,19 +7482,19 @@
         <v>77</v>
       </c>
       <c r="Q60" t="s">
+        <v>688</v>
+      </c>
+      <c r="R60" t="s">
         <v>689</v>
       </c>
-      <c r="R60" t="s">
+      <c r="S60" t="s">
+        <v>33</v>
+      </c>
+      <c r="T60" t="s">
+        <v>33</v>
+      </c>
+      <c r="U60" t="s">
         <v>690</v>
-      </c>
-      <c r="S60" t="s">
-        <v>33</v>
-      </c>
-      <c r="T60" t="s">
-        <v>33</v>
-      </c>
-      <c r="U60" t="s">
-        <v>691</v>
       </c>
       <c r="V60" t="s">
         <v>122</v>
@@ -7512,23 +7503,23 @@
         <v>205</v>
       </c>
       <c r="X60" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="Y60"/>
       <c r="Z60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>692</v>
+      </c>
+      <c r="B61" t="s">
+        <v>662</v>
+      </c>
+      <c r="C61" t="s">
         <v>693</v>
       </c>
-      <c r="B61" t="s">
-        <v>663</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>694</v>
-      </c>
-      <c r="D61" t="s">
-        <v>695</v>
       </c>
       <c r="E61" t="s">
         <v>52</v>
@@ -7543,16 +7534,16 @@
         <v>163</v>
       </c>
       <c r="I61" t="s">
+        <v>695</v>
+      </c>
+      <c r="J61" t="s">
         <v>696</v>
       </c>
-      <c r="J61" t="s">
+      <c r="K61" t="s">
+        <v>33</v>
+      </c>
+      <c r="L61" t="s">
         <v>697</v>
-      </c>
-      <c r="K61" t="s">
-        <v>33</v>
-      </c>
-      <c r="L61" t="s">
-        <v>698</v>
       </c>
       <c r="M61" t="s">
         <v>259</v>
@@ -7591,24 +7582,24 @@
         <v>46</v>
       </c>
       <c r="Y61" t="s">
+        <v>698</v>
+      </c>
+      <c r="Z61" t="s">
         <v>699</v>
-      </c>
-      <c r="Z61" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>700</v>
+      </c>
+      <c r="B62" t="s">
+        <v>662</v>
+      </c>
+      <c r="C62" t="s">
         <v>701</v>
       </c>
-      <c r="B62" t="s">
-        <v>663</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>702</v>
-      </c>
-      <c r="D62" t="s">
-        <v>703</v>
       </c>
       <c r="E62" t="s">
         <v>267</v>
@@ -7623,19 +7614,19 @@
         <v>33</v>
       </c>
       <c r="I62" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J62" t="s">
+        <v>703</v>
+      </c>
+      <c r="K62" t="s">
+        <v>33</v>
+      </c>
+      <c r="L62" t="s">
         <v>704</v>
       </c>
-      <c r="K62" t="s">
-        <v>33</v>
-      </c>
-      <c r="L62" t="s">
+      <c r="M62" t="s">
         <v>705</v>
-      </c>
-      <c r="M62" t="s">
-        <v>706</v>
       </c>
       <c r="N62" t="s">
         <v>89</v>
@@ -7647,11 +7638,11 @@
         <v>41</v>
       </c>
       <c r="Q62" t="s">
+        <v>706</v>
+      </c>
+      <c r="R62" t="s">
         <v>707</v>
       </c>
-      <c r="R62" t="s">
-        <v>708</v>
-      </c>
       <c r="S62" t="s">
         <v>33</v>
       </c>
@@ -7659,7 +7650,7 @@
         <v>33</v>
       </c>
       <c r="U62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V62" t="s">
         <v>92</v>
@@ -7671,24 +7662,24 @@
         <v>33</v>
       </c>
       <c r="Y62" t="s">
+        <v>708</v>
+      </c>
+      <c r="Z62" t="s">
         <v>709</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>710</v>
+      </c>
+      <c r="B63" t="s">
         <v>711</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>712</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>713</v>
-      </c>
-      <c r="D63" t="s">
-        <v>714</v>
       </c>
       <c r="E63" t="s">
         <v>52</v>
@@ -7703,19 +7694,19 @@
         <v>33</v>
       </c>
       <c r="I63" t="s">
+        <v>714</v>
+      </c>
+      <c r="J63" t="s">
         <v>715</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" t="s">
         <v>716</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" t="s">
         <v>717</v>
       </c>
-      <c r="L63" t="s">
-        <v>718</v>
-      </c>
       <c r="M63" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N63" t="s">
         <v>39</v>
@@ -7739,7 +7730,7 @@
         <v>33</v>
       </c>
       <c r="U63" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="V63" t="s">
         <v>33</v>
@@ -7751,22 +7742,22 @@
         <v>46</v>
       </c>
       <c r="Y63" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="Z63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>719</v>
+      </c>
+      <c r="B64" t="s">
+        <v>711</v>
+      </c>
+      <c r="C64" t="s">
         <v>720</v>
       </c>
-      <c r="B64" t="s">
-        <v>712</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>721</v>
-      </c>
-      <c r="D64" t="s">
-        <v>722</v>
       </c>
       <c r="E64" t="s">
         <v>52</v>
@@ -7775,22 +7766,22 @@
         <v>53</v>
       </c>
       <c r="G64" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H64" t="s">
         <v>269</v>
       </c>
       <c r="I64" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J64" t="s">
+        <v>723</v>
+      </c>
+      <c r="K64" t="s">
         <v>724</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>725</v>
-      </c>
-      <c r="L64" t="s">
-        <v>726</v>
       </c>
       <c r="M64" t="s">
         <v>59</v>
@@ -7817,7 +7808,7 @@
         <v>33</v>
       </c>
       <c r="U64" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V64" t="s">
         <v>62</v>
@@ -7829,28 +7820,28 @@
         <v>46</v>
       </c>
       <c r="Y64" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="Z64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>727</v>
+      </c>
+      <c r="B65" t="s">
+        <v>711</v>
+      </c>
+      <c r="C65" t="s">
         <v>728</v>
       </c>
-      <c r="B65" t="s">
-        <v>712</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>729</v>
-      </c>
-      <c r="D65" t="s">
-        <v>730</v>
       </c>
       <c r="E65" t="s">
         <v>52</v>
       </c>
       <c r="F65" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G65" t="s">
         <v>32</v>
@@ -7859,16 +7850,16 @@
         <v>33</v>
       </c>
       <c r="I65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J65" t="s">
+        <v>731</v>
+      </c>
+      <c r="K65" t="s">
         <v>732</v>
       </c>
-      <c r="K65" t="s">
-        <v>733</v>
-      </c>
       <c r="L65" t="s">
-        <v>734</v>
+        <v>537</v>
       </c>
       <c r="M65" t="s">
         <v>259</v>
@@ -7877,13 +7868,13 @@
         <v>39</v>
       </c>
       <c r="O65" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P65" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="Q65" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="R65" t="s">
         <v>33</v>
@@ -7895,7 +7886,7 @@
         <v>33</v>
       </c>
       <c r="U65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="V65" t="s">
         <v>45</v>
@@ -7907,27 +7898,27 @@
         <v>46</v>
       </c>
       <c r="Y65" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="Z65" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>736</v>
+      </c>
+      <c r="B66" t="s">
+        <v>737</v>
+      </c>
+      <c r="C66" t="s">
         <v>738</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>739</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>740</v>
-      </c>
-      <c r="D66" t="s">
-        <v>741</v>
-      </c>
-      <c r="E66" t="s">
-        <v>742</v>
       </c>
       <c r="F66" t="s">
         <v>53</v>
@@ -7939,25 +7930,25 @@
         <v>71</v>
       </c>
       <c r="I66" t="s">
+        <v>741</v>
+      </c>
+      <c r="J66" t="s">
+        <v>742</v>
+      </c>
+      <c r="K66" t="s">
+        <v>33</v>
+      </c>
+      <c r="L66" t="s">
         <v>743</v>
       </c>
-      <c r="J66" t="s">
+      <c r="M66" t="s">
         <v>744</v>
-      </c>
-      <c r="K66" t="s">
-        <v>33</v>
-      </c>
-      <c r="L66" t="s">
-        <v>745</v>
-      </c>
-      <c r="M66" t="s">
-        <v>746</v>
       </c>
       <c r="N66" t="s">
         <v>89</v>
       </c>
       <c r="O66" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="P66" t="s">
         <v>41</v>
@@ -7984,57 +7975,57 @@
         <v>205</v>
       </c>
       <c r="X66" t="s">
+        <v>745</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>746</v>
+      </c>
+      <c r="Z66" t="s">
         <v>747</v>
-      </c>
-      <c r="Y66" t="s">
-        <v>748</v>
-      </c>
-      <c r="Z66" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>748</v>
+      </c>
+      <c r="B67" t="s">
+        <v>749</v>
+      </c>
+      <c r="C67" t="s">
         <v>750</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>751</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
+        <v>480</v>
+      </c>
+      <c r="F67" t="s">
         <v>752</v>
       </c>
-      <c r="D67" t="s">
+      <c r="G67" t="s">
+        <v>33</v>
+      </c>
+      <c r="H67" t="s">
+        <v>33</v>
+      </c>
+      <c r="I67" t="s">
+        <v>449</v>
+      </c>
+      <c r="J67" t="s">
         <v>753</v>
       </c>
-      <c r="E67" t="s">
-        <v>481</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="K67" t="s">
+        <v>33</v>
+      </c>
+      <c r="L67" t="s">
         <v>754</v>
-      </c>
-      <c r="G67" t="s">
-        <v>33</v>
-      </c>
-      <c r="H67" t="s">
-        <v>33</v>
-      </c>
-      <c r="I67" t="s">
-        <v>450</v>
-      </c>
-      <c r="J67" t="s">
-        <v>755</v>
-      </c>
-      <c r="K67" t="s">
-        <v>33</v>
-      </c>
-      <c r="L67" t="s">
-        <v>756</v>
       </c>
       <c r="M67" t="s">
         <v>53</v>
       </c>
       <c r="N67" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="O67" t="s">
         <v>40</v>
@@ -8055,7 +8046,7 @@
         <v>33</v>
       </c>
       <c r="U67" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V67" t="s">
         <v>274</v>
@@ -8064,33 +8055,33 @@
         <v>205</v>
       </c>
       <c r="X67" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="Y67" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="Z67" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>758</v>
+      </c>
+      <c r="B68" t="s">
+        <v>749</v>
+      </c>
+      <c r="C68" t="s">
+        <v>759</v>
+      </c>
+      <c r="D68" t="s">
         <v>760</v>
       </c>
-      <c r="B68" t="s">
-        <v>751</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
         <v>761</v>
       </c>
-      <c r="D68" t="s">
+      <c r="F68" t="s">
         <v>762</v>
-      </c>
-      <c r="E68" t="s">
-        <v>763</v>
-      </c>
-      <c r="F68" t="s">
-        <v>764</v>
       </c>
       <c r="G68" t="s">
         <v>70</v>
@@ -8099,16 +8090,16 @@
         <v>71</v>
       </c>
       <c r="I68" t="s">
+        <v>763</v>
+      </c>
+      <c r="J68" t="s">
+        <v>764</v>
+      </c>
+      <c r="K68" t="s">
         <v>765</v>
       </c>
-      <c r="J68" t="s">
+      <c r="L68" t="s">
         <v>766</v>
-      </c>
-      <c r="K68" t="s">
-        <v>767</v>
-      </c>
-      <c r="L68" t="s">
-        <v>768</v>
       </c>
       <c r="M68" t="s">
         <v>53</v>
@@ -8144,30 +8135,30 @@
         <v>205</v>
       </c>
       <c r="X68" t="s">
+        <v>767</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>768</v>
+      </c>
+      <c r="Z68" t="s">
         <v>769</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>770</v>
-      </c>
-      <c r="Z68" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>770</v>
+      </c>
+      <c r="B69" t="s">
+        <v>771</v>
+      </c>
+      <c r="C69" t="s">
         <v>772</v>
       </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
         <v>773</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
         <v>774</v>
-      </c>
-      <c r="D69" t="s">
-        <v>775</v>
-      </c>
-      <c r="E69" t="s">
-        <v>776</v>
       </c>
       <c r="F69" t="s">
         <v>53</v>
@@ -8182,13 +8173,13 @@
         <v>270</v>
       </c>
       <c r="J69" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="K69" t="s">
         <v>33</v>
       </c>
       <c r="L69" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="M69" t="s">
         <v>38</v>
@@ -8203,7 +8194,7 @@
         <v>77</v>
       </c>
       <c r="Q69" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="R69" t="s">
         <v>33</v>
@@ -8224,25 +8215,25 @@
         <v>205</v>
       </c>
       <c r="X69" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="Y69" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="Z69"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>780</v>
+      </c>
+      <c r="B70" t="s">
+        <v>781</v>
+      </c>
+      <c r="C70" t="s">
         <v>782</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70" t="s">
         <v>783</v>
-      </c>
-      <c r="C70" t="s">
-        <v>784</v>
-      </c>
-      <c r="D70" t="s">
-        <v>785</v>
       </c>
       <c r="E70" t="s">
         <v>267</v>
@@ -8251,22 +8242,22 @@
         <v>53</v>
       </c>
       <c r="G70" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H70" t="s">
         <v>71</v>
       </c>
       <c r="I70" t="s">
+        <v>784</v>
+      </c>
+      <c r="J70" t="s">
+        <v>785</v>
+      </c>
+      <c r="K70" t="s">
         <v>786</v>
       </c>
-      <c r="J70" t="s">
+      <c r="L70" t="s">
         <v>787</v>
-      </c>
-      <c r="K70" t="s">
-        <v>788</v>
-      </c>
-      <c r="L70" t="s">
-        <v>789</v>
       </c>
       <c r="M70" t="s">
         <v>59</v>
@@ -8281,10 +8272,10 @@
         <v>41</v>
       </c>
       <c r="Q70" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="R70" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="S70" t="s">
         <v>33</v>
@@ -8305,24 +8296,24 @@
         <v>33</v>
       </c>
       <c r="Y70" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="Z70" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B71" t="s">
+        <v>781</v>
+      </c>
+      <c r="C71" t="s">
+        <v>782</v>
+      </c>
+      <c r="D71" t="s">
         <v>783</v>
-      </c>
-      <c r="C71" t="s">
-        <v>784</v>
-      </c>
-      <c r="D71" t="s">
-        <v>785</v>
       </c>
       <c r="E71" t="s">
         <v>267</v>
@@ -8331,22 +8322,22 @@
         <v>53</v>
       </c>
       <c r="G71" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="H71" t="s">
         <v>71</v>
       </c>
       <c r="I71" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="J71" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="K71" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="L71" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="M71" t="s">
         <v>59</v>
@@ -8361,7 +8352,7 @@
         <v>41</v>
       </c>
       <c r="Q71" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="R71" t="s">
         <v>33</v>
@@ -8385,10 +8376,10 @@
         <v>33</v>
       </c>
       <c r="Y71" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="Z71" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>